<commit_message>
add 1% check point
</commit_message>
<xml_diff>
--- a/result_format.xlsx
+++ b/result_format.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\SAR_image\noise2self\noise2self-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AEA105-38AE-4F37-8159-7F7ABDB9C7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F365F661-0DBA-4EA5-9BCE-1A4008C44B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11400" yWindow="3420" windowWidth="13620" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2790" yWindow="2625" windowWidth="21045" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="100%" sheetId="1" r:id="rId1"/>
     <sheet name="50%" sheetId="2" r:id="rId2"/>
     <sheet name="25%" sheetId="3" r:id="rId3"/>
     <sheet name="10%" sheetId="4" r:id="rId4"/>
+    <sheet name="1%" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="6">
   <si>
     <t>noise2void</t>
   </si>
@@ -5521,6 +5522,1155 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-DDC0-42A3-9C6F-197A5D0C2070}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="896709872"/>
+        <c:axId val="896710288"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="896709872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="896710288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="896710288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="896709872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:tint val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="104"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="4"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>PSNR</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'100%'!$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PNSR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:tint val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:tint val="65000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.3670166229221351E-4"/>
+                  <c:y val="-0.15141550014581509"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="ko-KR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'100%'!$C$10:$C$14998</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14989"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'100%'!$D$10:$D$14998</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14989"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FBF5-4692-8A22-0A8E7B91ADBA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="896709872"/>
+        <c:axId val="896710288"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="896709872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="896710288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="896710288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="896709872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:tint val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="108"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="8"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Loss</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'100%'!$E$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LOSS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:shade val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:shade val="65000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.3670166229221351E-4"/>
+                  <c:y val="-0.15141550014581509"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="ko-KR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'100%'!$C$10:$C$14998</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14989"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'100%'!$E$10:$E$14998</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14989"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A8E1-456C-88EF-10883E9D4CA4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="896709872"/>
+        <c:axId val="896710288"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="896709872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="896710288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="896710288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="896709872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:tint val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>V-Loss</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'100%'!$F$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>V-Loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:shade val="65000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.3670166229221351E-4"/>
+                  <c:y val="-0.15141550014581509"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="ko-KR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'100%'!$C$10:$C$14998</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14989"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'100%'!$F$10:$F$14998</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14989"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1BF3-48C3-95EB-1FEC48D85546}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9240,6 +10390,125 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>684609</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>684608</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A49CB50-BB8B-46A2-8BC3-C708CC6AB3CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>6654</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DC925CA-9F43-4374-9128-6D182FAF411D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>218280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>208358</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B33A181-1BCA-4908-8FA5-88EBB274BF62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
@@ -9822,7 +11091,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC2A569-42DB-45D0-B903-06BB00C2DA03}">
   <dimension ref="C1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -9911,4 +11182,99 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805A624F-6403-4556-BB66-5CA83AE99FB3}">
+  <dimension ref="C1:P9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="5.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="7" customWidth="1"/>
+    <col min="4" max="6" width="9" style="7"/>
+    <col min="7" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="3:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="3:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="H5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P5" s="2" t="str">
+        <f ca="1">MID(CELL("filename",A2),FIND("]",CELL("filename",A2))+1,255)</f>
+        <v>1%</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="3:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>